<commit_message>
Split categorization into keyflows
</commit_message>
<xml_diff>
--- a/Public_data/Exports_FW_part1/actor_roles_summary.xlsx
+++ b/Public_data/Exports_FW_part1/actor_roles_summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="201">
   <si>
     <t>Who</t>
   </si>
@@ -37,55 +37,337 @@
     <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar</t>
   </si>
   <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
     <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger</t>
   </si>
   <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Bemiddelaar, Bemiddelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Bemiddelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Handelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Ontvanger, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Bemiddelaar, Bemiddelaar, Handelaar, Handelaar, Handelaar, Handelaar, Handelaar, Handelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Bemiddelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Ontdoener, Ontdoener, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
     <t>Afzender, Afzender, Afzender, Afzender, Afzender, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar</t>
   </si>
   <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Bemiddelaar, Bemiddelaar, Bemiddelaar, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
     <t>Afzender, Afzender, Afzender, Afzender, Afzender, Bemiddelaar, Bemiddelaar, Handelaar</t>
   </si>
   <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Ontdoener, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Bemiddelaar, Ontvanger, Ontvanger, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Handelaar, Handelaar, Handelaar, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Handelaar, Handelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
     <t>Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Handelaar, Handelaar, Handelaar, Handelaar, Handelaar</t>
   </si>
   <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Handelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Ontvanger, Ontvanger, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontdoener, Ontdoener, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Afzender, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
     <t>Afzender, Afzender, Afzender, Afzender, Bemiddelaar, Bemiddelaar, Bemiddelaar</t>
   </si>
   <si>
     <t>Afzender, Afzender, Afzender, Afzender, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar</t>
   </si>
   <si>
-    <t>Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
+    <t>Afzender, Afzender, Afzender, Afzender, Bemiddelaar, Bemiddelaar, Bemiddelaar, Handelaar, Ontdoener, Ontdoener, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Bemiddelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger</t>
   </si>
   <si>
     <t>Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Bemiddelaar, Handelaar, Handelaar</t>
   </si>
   <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Inzamelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Afzender, Ontvanger, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
     <t>Afzender, Afzender, Afzender, Bemiddelaar, Bemiddelaar, Bemiddelaar</t>
   </si>
   <si>
+    <t>Afzender, Afzender, Afzender, Bemiddelaar, Bemiddelaar, Bemiddelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Bemiddelaar, Bemiddelaar, Bemiddelaar, Ontvanger, Ontdoener, Ontdoener, Herkomst, Herkomst</t>
+  </si>
+  <si>
     <t>Afzender, Afzender, Afzender, Handelaar, Handelaar, Handelaar</t>
   </si>
   <si>
+    <t>Afzender, Afzender, Afzender, Handelaar, Handelaar, Ontdoener, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Ontdoener, Ontdoener, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Inzamelaar, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Afzender, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
     <t>Afzender, Afzender, Bemiddelaar, Bemiddelaar</t>
   </si>
   <si>
-    <t>Afzender, Afzender, Bemiddelaar, Bemiddelaar, Handelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
+    <t>Afzender, Afzender, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Ontdoener, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Bemiddelaar, Bemiddelaar, Handelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Bemiddelaar, Bemiddelaar, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Bemiddelaar, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Bemiddelaar, Ontdoener, Herkomst</t>
   </si>
   <si>
     <t>Afzender, Afzender, Handelaar, Handelaar</t>
   </si>
   <si>
+    <t>Afzender, Afzender, Handelaar, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Handelaar, Ontdoener, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Bemiddelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontdoener, Ontdoener, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Inzamelaar, Inzamelaar, Ontdoener, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Inzamelaar, Inzamelaar, Ontdoener, Ontdoener, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Inzamelaar, Inzamelaar, Ontdoener, Ontdoener, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Inzamelaar, Ontdoener, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Inzamelaar, Ontdoener, Ontdoener, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Inzamelaar, Ontdoener, Ontdoener, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontdoener, Ontdoener, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Ontdoener, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Ontdoener, Ontdoener, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Ontdoener, Ontdoener, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Afzender, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
     <t>Afzender, Bemiddelaar</t>
   </si>
   <si>
-    <t>Afzender, Bemiddelaar, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Afzender, Bemiddelaar, Verwerker</t>
-  </si>
-  <si>
-    <t>Afzender, Bemiddelaar, Verwerker, Verwerker</t>
+    <t>Afzender, Bemiddelaar, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Bemiddelaar, Ontdoener, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Bemiddelaar, Ontdoener, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Bemiddelaar, Ontvanger</t>
+  </si>
+  <si>
+    <t>Afzender, Bemiddelaar, Ontvanger, Ontdoener, Herkomst</t>
   </si>
   <si>
     <t>Afzender, Handelaar</t>
@@ -94,13 +376,67 @@
     <t>Afzender, Inzamelaar, Bemiddelaar</t>
   </si>
   <si>
-    <t>Afzender, Inzamelaar, Bemiddelaar, Ontvanger, Verwerker</t>
+    <t>Afzender, Inzamelaar, Bemiddelaar, Ontvanger</t>
   </si>
   <si>
     <t>Afzender, Inzamelaar, Inzamelaar, Bemiddelaar</t>
   </si>
   <si>
-    <t>Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
+    <t>Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger</t>
+  </si>
+  <si>
+    <t>Afzender, Inzamelaar, Inzamelaar, Ontdoener, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Inzamelaar, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Inzamelaar, Ontdoener, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Inzamelaar, Ontdoener, Ontdoener, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Inzamelaar, Ontvanger, Ontdoener, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontdoener, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Ontdoener, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Ontdoener, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Ontdoener, Ontdoener, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Ontdoener, Ontdoener, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Ontdoener, Ontdoener, Ontdoener</t>
+  </si>
+  <si>
+    <t>Afzender, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Ontvanger, Ontdoener, Herkomst</t>
+  </si>
+  <si>
+    <t>Afzender, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontdoener, Herkomst</t>
   </si>
   <si>
     <t>Herkomst</t>
@@ -109,9 +445,6 @@
     <t>Herkomst, Herkomst</t>
   </si>
   <si>
-    <t>Herkomst, Herkomst, Afzender, Afzender, Bemiddelaar, Bemiddelaar</t>
-  </si>
-  <si>
     <t>Herkomst, Herkomst, Herkomst</t>
   </si>
   <si>
@@ -124,12 +457,6 @@
     <t>Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
   </si>
   <si>
-    <t>Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Herkomst, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
     <t>Inzamelaar</t>
   </si>
   <si>
@@ -145,22 +472,25 @@
     <t>Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar</t>
   </si>
   <si>
+    <t>Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
+  </si>
+  <si>
     <t>Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger</t>
   </si>
   <si>
     <t>Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger</t>
   </si>
   <si>
-    <t>Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger, Verwerker</t>
+    <t>Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener</t>
+  </si>
+  <si>
+    <t>Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger</t>
+  </si>
+  <si>
+    <t>Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger</t>
+  </si>
+  <si>
+    <t>Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger</t>
   </si>
   <si>
     <t>Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger</t>
@@ -169,438 +499,87 @@
     <t>Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontvanger</t>
   </si>
   <si>
-    <t>Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Verwerker, Verwerker</t>
+    <t>Inzamelaar, Inzamelaar, Ontdoener, Ontdoener, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Inzamelaar, Inzamelaar, Ontvanger, Ontvanger</t>
+  </si>
+  <si>
+    <t>Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontdoener, Ontdoener, Herkomst, Herkomst</t>
+  </si>
+  <si>
+    <t>Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger</t>
+  </si>
+  <si>
+    <t>Inzamelaar, Ontdoener, Herkomst</t>
+  </si>
+  <si>
+    <t>Inzamelaar, Ontvanger</t>
+  </si>
+  <si>
+    <t>Inzamelaar, Ontvanger, Ontvanger, Ontvanger</t>
   </si>
   <si>
     <t>Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger</t>
   </si>
   <si>
-    <t>Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Inzamelaar, Ontvanger, Verwerker</t>
-  </si>
-  <si>
     <t>Ontdoener</t>
   </si>
   <si>
-    <t>Ontdoener, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Handelaar, Handelaar, Handelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Afzender, Afzender, Bemiddelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Afzender, Afzender, Handelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Afzender, Bemiddelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Afzender, Inzamelaar</t>
-  </si>
-  <si>
     <t>Ontdoener, Herkomst</t>
   </si>
   <si>
-    <t>Ontdoener, Herkomst, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Herkomst, Afzender, Afzender, Bemiddelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Herkomst, Afzender, Afzender, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Herkomst, Afzender, Afzender, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Herkomst, Afzender, Bemiddelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Herkomst, Afzender, Bemiddelaar, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Ontdoener, Herkomst, Afzender, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Herkomst, Afzender, Inzamelaar, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Herkomst, Afzender, Inzamelaar, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Ontdoener, Herkomst, Afzender, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger</t>
-  </si>
-  <si>
-    <t>Ontdoener, Herkomst, Afzender, Ontvanger, Verwerker</t>
-  </si>
-  <si>
-    <t>Ontdoener, Herkomst, Afzender, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Ontdoener, Herkomst, Herkomst, Afzender, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger</t>
-  </si>
-  <si>
-    <t>Ontdoener, Herkomst, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Herkomst, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
     <t>Ontdoener, Ontdoener</t>
   </si>
   <si>
-    <t>Ontdoener, Ontdoener, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Afzender, Afzender, Afzender, Handelaar, Handelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Afzender, Afzender, Handelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Afzender, Afzender, Inzamelaar, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Afzender, Bemiddelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Herkomst, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Herkomst, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Herkomst, Afzender, Afzender, Afzender, Afzender, Bemiddelaar, Bemiddelaar, Bemiddelaar, Handelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Herkomst, Afzender, Afzender, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Herkomst, Afzender, Afzender, Inzamelaar, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Herkomst, Afzender, Inzamelaar</t>
-  </si>
-  <si>
     <t>Ontdoener, Ontdoener, Herkomst, Herkomst</t>
   </si>
   <si>
-    <t>Ontdoener, Ontdoener, Herkomst, Herkomst, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Herkomst, Herkomst, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Ontvanger, Ontvanger, Ontvanger, Ontvanger</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Herkomst, Herkomst, Afzender, Afzender, Afzender, Bemiddelaar, Bemiddelaar, Bemiddelaar, Ontvanger</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Herkomst, Herkomst, Afzender, Afzender, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Herkomst, Herkomst, Afzender, Afzender, Inzamelaar, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Herkomst, Herkomst, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Herkomst, Herkomst, Afzender, Afzender, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Herkomst, Herkomst, Inzamelaar, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Herkomst, Herkomst, Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
     <t>Ontdoener, Ontdoener, Ontdoener</t>
   </si>
   <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Afzender, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Herkomst, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
     <t>Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst</t>
   </si>
   <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Ontvanger, Verwerker</t>
-  </si>
-  <si>
     <t>Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst</t>
   </si>
   <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Bemiddelaar, Bemiddelaar, Bemiddelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Handelaar, Handelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
     <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener</t>
   </si>
   <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Afzender, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
     <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst</t>
   </si>
   <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Bemiddelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Ontvanger</t>
-  </si>
-  <si>
     <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener</t>
   </si>
   <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Afzender, Afzender, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Afzender, Afzender, Afzender, Bemiddelaar, Bemiddelaar, Bemiddelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar</t>
-  </si>
-  <si>
     <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst</t>
   </si>
   <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Bemiddelaar, Ontvanger, Ontvanger, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
     <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
   </si>
   <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Handelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Ontvanger, Ontvanger, Verwerker, Verwerker</t>
-  </si>
-  <si>
     <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener</t>
   </si>
   <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Bemiddelaar</t>
-  </si>
-  <si>
     <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst</t>
   </si>
   <si>
     <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst</t>
   </si>
   <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
     <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
   </si>
   <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar</t>
-  </si>
-  <si>
     <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
   </si>
   <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Bemiddelaar, Bemiddelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Handelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Bemiddelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Bemiddelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Bemiddelaar, Bemiddelaar, Handelaar, Handelaar, Handelaar, Handelaar, Handelaar, Handelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Afzender, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Afzender, Afzender, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Bemiddelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar</t>
-  </si>
-  <si>
-    <t>Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Ontdoener, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Inzamelaar, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
     <t>Ontvanger</t>
   </si>
   <si>
+    <t>Ontvanger, Herkomst</t>
+  </si>
+  <si>
     <t>Ontvanger, Ontvanger</t>
   </si>
   <si>
@@ -610,37 +589,16 @@
     <t>Ontvanger, Ontvanger, Ontvanger, Ontvanger</t>
   </si>
   <si>
+    <t>Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontdoener, Herkomst</t>
+  </si>
+  <si>
     <t>Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger</t>
   </si>
   <si>
     <t>Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger</t>
   </si>
   <si>
-    <t>Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Ontvanger, Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Ontvanger, Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Ontvanger, Ontvanger, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Ontvanger, Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Ontvanger, Verwerker</t>
-  </si>
-  <si>
-    <t>Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
-  </si>
-  <si>
-    <t>Ontvanger, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker, Verwerker</t>
+    <t>Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Ontvanger, Herkomst, Herkomst, Herkomst, Herkomst, Herkomst</t>
   </si>
   <si>
     <t>Verwerker</t>
@@ -1016,7 +974,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B215"/>
+  <dimension ref="A1:B201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1091,7 +1049,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1107,7 +1065,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1115,7 +1073,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1123,7 +1081,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1147,7 +1105,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1163,7 +1121,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1179,7 +1137,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1187,7 +1145,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1195,7 +1153,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1219,7 +1177,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1243,7 +1201,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1251,7 +1209,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1259,7 +1217,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>273</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1267,7 +1225,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>66</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1283,7 +1241,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1291,7 +1249,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1299,7 +1257,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1307,7 +1265,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>29</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1331,7 +1289,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1339,7 +1297,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1347,7 +1305,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1355,7 +1313,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1387,7 +1345,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1403,7 +1361,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1411,7 +1369,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1419,7 +1377,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1427,7 +1385,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1435,7 +1393,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1459,7 +1417,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1467,7 +1425,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1475,7 +1433,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>49</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1483,7 +1441,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>82</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1499,7 +1457,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1523,7 +1481,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1531,7 +1489,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>135</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1539,7 +1497,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>309</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1547,7 +1505,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>1</v>
+        <v>36</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1571,7 +1529,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1595,7 +1553,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>45</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1611,7 +1569,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1619,7 +1577,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1635,7 +1593,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1651,7 +1609,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1659,7 +1617,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>1</v>
+        <v>59</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1667,7 +1625,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1675,7 +1633,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1683,7 +1641,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1715,7 +1673,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1723,7 +1681,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1731,7 +1689,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1755,7 +1713,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1763,7 +1721,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1779,7 +1737,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>52</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1787,7 +1745,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1795,7 +1753,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>104</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1851,7 +1809,7 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1867,7 +1825,7 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1875,7 +1833,7 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1883,7 +1841,7 @@
         <v>107</v>
       </c>
       <c r="B108">
-        <v>1</v>
+        <v>104</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1891,7 +1849,7 @@
         <v>108</v>
       </c>
       <c r="B109">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1899,7 +1857,7 @@
         <v>109</v>
       </c>
       <c r="B110">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1907,7 +1865,7 @@
         <v>110</v>
       </c>
       <c r="B111">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1915,7 +1873,7 @@
         <v>111</v>
       </c>
       <c r="B112">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1923,7 +1881,7 @@
         <v>112</v>
       </c>
       <c r="B113">
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1947,7 +1905,7 @@
         <v>115</v>
       </c>
       <c r="B116">
-        <v>28</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1955,7 +1913,7 @@
         <v>116</v>
       </c>
       <c r="B117">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1963,7 +1921,7 @@
         <v>117</v>
       </c>
       <c r="B118">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1971,7 +1929,7 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>59</v>
+        <v>10</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2003,7 +1961,7 @@
         <v>122</v>
       </c>
       <c r="B123">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2011,7 +1969,7 @@
         <v>123</v>
       </c>
       <c r="B124">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2019,7 +1977,7 @@
         <v>124</v>
       </c>
       <c r="B125">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -2027,7 +1985,7 @@
         <v>125</v>
       </c>
       <c r="B126">
-        <v>4</v>
+        <v>45</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -2035,7 +1993,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2051,7 +2009,7 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2059,7 +2017,7 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>18</v>
+        <v>82</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2067,7 +2025,7 @@
         <v>130</v>
       </c>
       <c r="B131">
-        <v>1</v>
+        <v>310</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -2091,7 +2049,7 @@
         <v>133</v>
       </c>
       <c r="B134">
-        <v>36</v>
+        <v>7</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -2099,7 +2057,7 @@
         <v>134</v>
       </c>
       <c r="B135">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -2107,7 +2065,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2123,7 +2081,7 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2131,7 +2089,7 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2147,7 +2105,7 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2155,7 +2113,7 @@
         <v>141</v>
       </c>
       <c r="B142">
-        <v>1</v>
+        <v>273</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2163,7 +2121,7 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>1</v>
+        <v>66</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2171,7 +2129,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2179,7 +2137,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2187,7 +2145,7 @@
         <v>145</v>
       </c>
       <c r="B146">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2195,7 +2153,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2203,7 +2161,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2211,7 +2169,7 @@
         <v>148</v>
       </c>
       <c r="B149">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2219,7 +2177,7 @@
         <v>149</v>
       </c>
       <c r="B150">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2227,7 +2185,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2243,7 +2201,7 @@
         <v>152</v>
       </c>
       <c r="B153">
-        <v>42</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -2259,7 +2217,7 @@
         <v>154</v>
       </c>
       <c r="B155">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -2283,7 +2241,7 @@
         <v>157</v>
       </c>
       <c r="B158">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -2291,7 +2249,7 @@
         <v>158</v>
       </c>
       <c r="B159">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -2307,7 +2265,7 @@
         <v>160</v>
       </c>
       <c r="B161">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -2315,7 +2273,7 @@
         <v>161</v>
       </c>
       <c r="B162">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -2323,7 +2281,7 @@
         <v>162</v>
       </c>
       <c r="B163">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -2331,7 +2289,7 @@
         <v>163</v>
       </c>
       <c r="B164">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -2339,7 +2297,7 @@
         <v>164</v>
       </c>
       <c r="B165">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -2347,7 +2305,7 @@
         <v>165</v>
       </c>
       <c r="B166">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -2355,7 +2313,7 @@
         <v>166</v>
       </c>
       <c r="B167">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -2379,7 +2337,7 @@
         <v>169</v>
       </c>
       <c r="B170">
-        <v>1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -2387,7 +2345,7 @@
         <v>170</v>
       </c>
       <c r="B171">
-        <v>83</v>
+        <v>135</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -2395,7 +2353,7 @@
         <v>171</v>
       </c>
       <c r="B172">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -2403,7 +2361,7 @@
         <v>172</v>
       </c>
       <c r="B173">
-        <v>2</v>
+        <v>52</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -2411,7 +2369,7 @@
         <v>173</v>
       </c>
       <c r="B174">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -2419,7 +2377,7 @@
         <v>174</v>
       </c>
       <c r="B175">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -2427,7 +2385,7 @@
         <v>175</v>
       </c>
       <c r="B176">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -2435,7 +2393,7 @@
         <v>176</v>
       </c>
       <c r="B177">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -2443,7 +2401,7 @@
         <v>177</v>
       </c>
       <c r="B178">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -2451,7 +2409,7 @@
         <v>178</v>
       </c>
       <c r="B179">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -2459,7 +2417,7 @@
         <v>179</v>
       </c>
       <c r="B180">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -2467,7 +2425,7 @@
         <v>180</v>
       </c>
       <c r="B181">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -2475,7 +2433,7 @@
         <v>181</v>
       </c>
       <c r="B182">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -2483,7 +2441,7 @@
         <v>182</v>
       </c>
       <c r="B183">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -2507,7 +2465,7 @@
         <v>185</v>
       </c>
       <c r="B186">
-        <v>1</v>
+        <v>83</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -2515,7 +2473,7 @@
         <v>186</v>
       </c>
       <c r="B187">
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="188" spans="1:2">
@@ -2531,7 +2489,7 @@
         <v>188</v>
       </c>
       <c r="B189">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="190" spans="1:2">
@@ -2539,7 +2497,7 @@
         <v>189</v>
       </c>
       <c r="B190">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -2547,7 +2505,7 @@
         <v>190</v>
       </c>
       <c r="B191">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -2563,7 +2521,7 @@
         <v>192</v>
       </c>
       <c r="B193">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -2571,7 +2529,7 @@
         <v>193</v>
       </c>
       <c r="B194">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -2579,7 +2537,7 @@
         <v>194</v>
       </c>
       <c r="B195">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -2587,7 +2545,7 @@
         <v>195</v>
       </c>
       <c r="B196">
-        <v>4</v>
+        <v>69</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -2595,7 +2553,7 @@
         <v>196</v>
       </c>
       <c r="B197">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -2603,7 +2561,7 @@
         <v>197</v>
       </c>
       <c r="B198">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -2611,7 +2569,7 @@
         <v>198</v>
       </c>
       <c r="B199">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -2619,7 +2577,7 @@
         <v>199</v>
       </c>
       <c r="B200">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -2627,119 +2585,7 @@
         <v>200</v>
       </c>
       <c r="B201">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2">
-      <c r="A202" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B202">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2">
-      <c r="A203" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B203">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2">
-      <c r="A204" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B204">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2">
-      <c r="A205" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B205">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2">
-      <c r="A206" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B206">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2">
-      <c r="A207" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B207">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2">
-      <c r="A208" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B208">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2">
-      <c r="A209" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B209">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2">
-      <c r="A210" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B210">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2">
-      <c r="A211" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B211">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2">
-      <c r="A212" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B212">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2">
-      <c r="A213" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B213">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2">
-      <c r="A214" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B214">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2">
-      <c r="A215" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B215">
-        <v>7</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>